<commit_message>
Aggiunta gestione annunci pubblicitari
</commit_message>
<xml_diff>
--- a/data_input.xlsx
+++ b/data_input.xlsx
@@ -557,8 +557,8 @@
           <t>SI</t>
         </is>
       </c>
-      <c r="N2" s="2" t="n">
-        <v>45908</v>
+      <c r="N2" s="3" t="n">
+        <v>45909</v>
       </c>
       <c r="O2" t="inlineStr"/>
     </row>
@@ -612,8 +612,8 @@
           <t>SI</t>
         </is>
       </c>
-      <c r="N3" s="2" t="n">
-        <v>45908</v>
+      <c r="N3" s="3" t="n">
+        <v>45909</v>
       </c>
       <c r="O3" t="inlineStr"/>
     </row>
@@ -658,7 +658,7 @@
         </is>
       </c>
       <c r="N4" s="3" t="n">
-        <v>45908</v>
+        <v>45909</v>
       </c>
       <c r="O4" t="inlineStr"/>
     </row>

</xml_diff>

<commit_message>
Tutti i prezzi impostati come valoure numerico
</commit_message>
<xml_diff>
--- a/data_input.xlsx
+++ b/data_input.xlsx
@@ -558,7 +558,7 @@
         </is>
       </c>
       <c r="N2" s="3" t="n">
-        <v>45909</v>
+        <v>45911</v>
       </c>
       <c r="O2" t="inlineStr"/>
     </row>
@@ -613,7 +613,7 @@
         </is>
       </c>
       <c r="N3" s="3" t="n">
-        <v>45909</v>
+        <v>45911</v>
       </c>
       <c r="O3" t="inlineStr"/>
     </row>
@@ -658,7 +658,7 @@
         </is>
       </c>
       <c r="N4" s="3" t="n">
-        <v>45909</v>
+        <v>45911</v>
       </c>
       <c r="O4" t="inlineStr"/>
     </row>

</xml_diff>

<commit_message>
Aggiunto avviso e minor changes
</commit_message>
<xml_diff>
--- a/data_input.xlsx
+++ b/data_input.xlsx
@@ -558,7 +558,7 @@
         </is>
       </c>
       <c r="N2" s="3" t="n">
-        <v>45911</v>
+        <v>45912</v>
       </c>
       <c r="O2" t="inlineStr"/>
     </row>
@@ -613,7 +613,7 @@
         </is>
       </c>
       <c r="N3" s="3" t="n">
-        <v>45911</v>
+        <v>45912</v>
       </c>
       <c r="O3" t="inlineStr"/>
     </row>
@@ -658,7 +658,7 @@
         </is>
       </c>
       <c r="N4" s="3" t="n">
-        <v>45911</v>
+        <v>45912</v>
       </c>
       <c r="O4" t="inlineStr"/>
     </row>

</xml_diff>